<commit_message>
Created Buttons on FormNMBS to get TC widths and wood requirements from Joist Details.
</commit_message>
<xml_diff>
--- a/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
+++ b/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop 2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="9708"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="9705"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,7 +346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -365,7 +360,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
Wood Nailer Briding and Bolts
</commit_message>
<xml_diff>
--- a/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
+++ b/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darien.shannon\Desktop\DESign\DESign\DESign_BOT\DESign_BOT\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darien.shannon\code\DESign\DESign_BOT\DESign_BOT\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Pattern:</t>
   </si>
@@ -38,9 +38,6 @@
     <t>B:</t>
   </si>
   <si>
-    <t>Non-Staggered</t>
-  </si>
-  <si>
     <t>HC:</t>
   </si>
   <si>
@@ -48,6 +45,15 @@
   </si>
   <si>
     <t>MARKS:</t>
+  </si>
+  <si>
+    <t>Wood Thickness:</t>
+  </si>
+  <si>
+    <t>3x</t>
+  </si>
+  <si>
+    <t>Staggered</t>
   </si>
 </sst>
 </file>
@@ -400,15 +406,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I5"/>
+  <dimension ref="B2:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -423,33 +430,44 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
-      <formula1>"Non-Staggered,Staggered"</formula1>
+      <formula1>"Staggered,Non-Staggered"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+      <formula1>"3x,2"""</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Panelized Job option
</commit_message>
<xml_diff>
--- a/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
+++ b/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Pattern:</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Staggered</t>
+  </si>
+  <si>
+    <t>Panelized Job?</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -86,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -94,14 +100,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I6"/>
+  <dimension ref="B1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -420,25 +494,35 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -462,12 +546,15 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>"Staggered,Non-Staggered"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
       <formula1>"3x,2"""</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Work on Wood Nailer Sheet
</commit_message>
<xml_diff>
--- a/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
+++ b/DESign_BOT/DESign_BOT/Resources/BLANK_AB_SHEET.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darien.shannon\code\DESign\DESign_BOT\DESign_BOT\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darien.shannon\Documents\Code\DESign\DESign_BOT\DESign_BOT\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD460DC-8A83-407F-A855-BF0078479052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Pattern:</t>
   </si>
@@ -60,12 +61,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Crimped Webs</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -162,11 +169,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -176,6 +209,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -269,6 +304,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -304,6 +356,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,11 +548,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +560,8 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -501,7 +571,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -509,12 +579,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -547,13 +623,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Staggered,Non-Staggered"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"3x,2"""</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 E4" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -563,7 +639,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -575,7 +651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>